<commit_message>
read setting-data from CSV!
</commit_message>
<xml_diff>
--- a/配列.xlsx
+++ b/配列.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yamaguchisouta/RBC/ATEM_Controller/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yamaguchisouta/RBC/Dev_ATEM-Controller/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BACE54E1-94AF-6249-A6F3-12E14E7E7877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7686690-F897-294F-997E-F5586D7DD481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="1200" windowWidth="28300" windowHeight="17440" xr2:uid="{86AB5C92-71B4-9F4A-94AA-B2EEC83C878C}"/>
+    <workbookView xWindow="4380" yWindow="1200" windowWidth="28300" windowHeight="17440" activeTab="1" xr2:uid="{86AB5C92-71B4-9F4A-94AA-B2EEC83C878C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="80">
   <si>
     <t>4A</t>
     <phoneticPr fontId="1"/>
@@ -296,6 +297,50 @@
   <si>
     <t>Color2</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>M/E1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>M/E2</t>
+  </si>
+  <si>
+    <t>M/E3</t>
+  </si>
+  <si>
+    <t>M/E4</t>
+  </si>
+  <si>
+    <t>Mode1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mode2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BKGD</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KEY1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KEY2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KEY3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>KEY4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ON AIR</t>
   </si>
 </sst>
 </file>
@@ -337,7 +382,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,8 +425,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA4AB"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6FFB6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="52">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -998,6 +1055,135 @@
       <right/>
       <top/>
       <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1008,7 +1194,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1021,9 +1207,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1045,19 +1228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1240,24 +1411,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1270,9 +1429,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1304,12 +1460,6 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1326,6 +1476,156 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="62" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1335,8 +1635,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFB6FFB6"/>
+      <color rgb="FF7FFF7F"/>
+      <color rgb="FFFFA4AB"/>
       <color rgb="FFFF7F88"/>
-      <color rgb="FF7FFF7F"/>
       <color rgb="FF78D0F0"/>
       <color rgb="FFFF5964"/>
     </mruColors>
@@ -1651,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF722458-58E1-F844-BAB5-D0E757015CDB}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1"/>
@@ -1663,530 +1965,1091 @@
     <row r="1" spans="1:15" ht="30" customHeight="1" thickBot="1"/>
     <row r="2" spans="1:15" ht="30" customHeight="1" thickTop="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="78" t="s">
+      <c r="C2" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="78" t="s">
+      <c r="E2" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="78" t="s">
+      <c r="F2" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="78">
+      <c r="G2" s="72">
         <v>60</v>
       </c>
-      <c r="H2" s="78">
+      <c r="H2" s="72">
         <v>61</v>
       </c>
-      <c r="I2" s="79">
+      <c r="I2" s="73">
         <v>62</v>
       </c>
-      <c r="J2" s="99">
+      <c r="J2" s="94">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="30" customHeight="1" thickBot="1">
       <c r="A3" s="2"/>
-      <c r="B3" s="80"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="113" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="100"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
+      <c r="F3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="95"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1" thickTop="1">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>51</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>52</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>53</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>54</v>
       </c>
-      <c r="F4" s="73">
+      <c r="F4" s="68">
         <v>55</v>
       </c>
-      <c r="G4" s="71">
+      <c r="G4" s="66">
         <v>56</v>
       </c>
-      <c r="H4" s="42">
+      <c r="H4" s="96">
         <v>57</v>
       </c>
-      <c r="I4" s="43">
+      <c r="I4" s="97">
         <v>58</v>
       </c>
-      <c r="J4" s="81">
+      <c r="J4" s="98">
         <v>59</v>
       </c>
-      <c r="L4" s="34">
+      <c r="L4" s="29">
         <v>5</v>
       </c>
-      <c r="M4" s="35">
+      <c r="M4" s="30">
         <v>7</v>
       </c>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1">
       <c r="A5" s="2"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="74" t="s">
+      <c r="F5" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="14" t="s">
+      <c r="G5" s="22"/>
+      <c r="H5" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="I5" s="28" t="s">
+      <c r="I5" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="J5" s="82" t="s">
+      <c r="J5" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="L5" s="36">
+      <c r="L5" s="31">
         <v>15</v>
       </c>
-      <c r="M5" s="35">
+      <c r="M5" s="30">
         <v>17</v>
       </c>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
     </row>
     <row r="6" spans="1:15" ht="30" customHeight="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>47</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>48</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>49</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="75" t="s">
+      <c r="F6" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="46" t="s">
+      <c r="G6" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="102" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="83" t="s">
+      <c r="J6" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="37">
+      <c r="L6" s="32">
         <v>9</v>
       </c>
-      <c r="M6" s="35" t="s">
+      <c r="M6" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1" thickBot="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="76" t="s">
+      <c r="B7" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="E7" s="62" t="s">
+      <c r="E7" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="63" t="s">
+      <c r="F7" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="72"/>
-      <c r="H7" s="15" t="s">
+      <c r="G7" s="67"/>
+      <c r="H7" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="100" t="s">
         <v>67</v>
       </c>
-      <c r="J7" s="84" t="s">
+      <c r="J7" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="38">
+      <c r="L7" s="33">
         <v>22</v>
       </c>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
     </row>
     <row r="8" spans="1:15" ht="30" customHeight="1">
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="16">
         <v>40</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="25">
         <v>41</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="24">
         <v>42</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>43</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="21">
         <v>44</v>
       </c>
-      <c r="J8" s="85">
+      <c r="J8" s="76">
         <v>45</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="30">
         <v>3</v>
       </c>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
     </row>
     <row r="9" spans="1:15" ht="30" customHeight="1" thickBot="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="86" t="s">
+      <c r="B9" s="42"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="77" t="s">
         <v>50</v>
       </c>
-      <c r="L9" s="105" t="s">
+      <c r="L9" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
     </row>
     <row r="10" spans="1:15" ht="30" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="44">
+      <c r="B10" s="39">
         <v>33</v>
       </c>
-      <c r="C10" s="45">
+      <c r="C10" s="40">
         <v>34</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="40">
         <v>35</v>
       </c>
-      <c r="E10" s="45">
+      <c r="E10" s="40">
         <v>36</v>
       </c>
-      <c r="F10" s="49">
+      <c r="F10" s="44">
         <v>37</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="41">
         <v>38</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H10" s="105">
         <v>39</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="106" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="87" t="s">
+      <c r="J10" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
     </row>
     <row r="11" spans="1:15" ht="30" customHeight="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="65"/>
-      <c r="H11" s="15" t="s">
+      <c r="G11" s="60"/>
+      <c r="H11" s="108" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="J11" s="82" t="s">
+      <c r="J11" s="110" t="s">
         <v>51</v>
       </c>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
     </row>
     <row r="12" spans="1:15" ht="30" customHeight="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="17">
+      <c r="B12" s="12">
         <v>29</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="51" t="s">
+      <c r="F12" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="66" t="s">
+      <c r="G12" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="H12" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="106">
         <v>30</v>
       </c>
-      <c r="J12" s="56">
+      <c r="J12" s="111">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="30" customHeight="1" thickBot="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="54" t="s">
+      <c r="B13" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="52" t="s">
+      <c r="D13" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="53" t="s">
+      <c r="F13" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="14" t="s">
+      <c r="G13" s="22"/>
+      <c r="H13" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="109" t="s">
         <v>67</v>
       </c>
-      <c r="J13" s="56" t="s">
+      <c r="J13" s="111" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="30" customHeight="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="16">
         <v>20</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="25">
         <v>21</v>
       </c>
-      <c r="E14" s="39">
+      <c r="E14" s="34">
         <v>22</v>
       </c>
-      <c r="F14" s="21">
+      <c r="F14" s="16">
         <v>23</v>
       </c>
-      <c r="G14" s="41">
+      <c r="G14" s="36">
         <v>24</v>
       </c>
-      <c r="H14" s="21">
+      <c r="H14" s="16">
         <v>25</v>
       </c>
-      <c r="I14" s="26">
+      <c r="I14" s="21">
         <v>26</v>
       </c>
-      <c r="J14" s="56">
+      <c r="J14" s="51">
         <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="30" customHeight="1" thickBot="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="56"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="51"/>
     </row>
     <row r="16" spans="1:15" ht="30" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="101">
+      <c r="B16" s="89">
         <v>15</v>
       </c>
-      <c r="C16" s="58">
+      <c r="C16" s="53">
         <v>16</v>
       </c>
-      <c r="D16" s="59">
+      <c r="D16" s="54">
         <v>17</v>
       </c>
-      <c r="E16" s="91">
+      <c r="E16" s="81">
         <v>18</v>
       </c>
-      <c r="F16" s="57">
+      <c r="F16" s="52">
         <v>19</v>
       </c>
-      <c r="G16" s="95" t="s">
+      <c r="G16" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="96" t="s">
+      <c r="H16" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="97" t="s">
+      <c r="I16" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="98" t="s">
+      <c r="J16" s="88" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="102" t="s">
+      <c r="B17" s="90" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="60" t="s">
+      <c r="D17" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="92"/>
-      <c r="F17" s="31" t="s">
+      <c r="E17" s="82"/>
+      <c r="F17" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="55" t="s">
+      <c r="H17" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="I17" s="33" t="s">
+      <c r="I17" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="J17" s="88" t="s">
+      <c r="J17" s="78" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="2"/>
-      <c r="B18" s="103" t="s">
+      <c r="B18" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="93" t="s">
+      <c r="E18" s="83" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="67">
+      <c r="G18" s="62">
         <v>10</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <v>11</v>
       </c>
-      <c r="I18" s="68">
+      <c r="I18" s="63">
         <v>12</v>
       </c>
-      <c r="J18" s="89">
+      <c r="J18" s="79">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30" customHeight="1" thickBot="1">
       <c r="A19" s="2"/>
-      <c r="B19" s="104" t="s">
+      <c r="B19" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="94"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="69" t="s">
+      <c r="E19" s="84"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="70" t="s">
+      <c r="H19" s="20"/>
+      <c r="I19" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="90" t="s">
+      <c r="J19" s="80" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" customHeight="1" thickTop="1"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J2:J3"/>
+  </mergeCells>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{325BCFAD-08CF-6041-B676-A3A0860CFA73}">
+  <dimension ref="A1:O20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1"/>
+  <cols>
+    <col min="1" max="16384" width="10.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="30" customHeight="1" thickBot="1"/>
+    <row r="2" spans="1:15" ht="30" customHeight="1" thickTop="1">
+      <c r="A2" s="2"/>
+      <c r="B2" s="116" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="114" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="72" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="72">
+        <v>60</v>
+      </c>
+      <c r="H2" s="72">
+        <v>61</v>
+      </c>
+      <c r="I2" s="73">
+        <v>62</v>
+      </c>
+      <c r="J2" s="94">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="30" customHeight="1" thickBot="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="115" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="95"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+    </row>
+    <row r="4" spans="1:15" ht="30" customHeight="1" thickTop="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="116">
+        <v>51</v>
+      </c>
+      <c r="C4" s="37">
+        <v>52</v>
+      </c>
+      <c r="D4" s="124">
+        <v>53</v>
+      </c>
+      <c r="E4" s="127">
+        <v>54</v>
+      </c>
+      <c r="F4" s="37">
+        <v>55</v>
+      </c>
+      <c r="G4" s="66">
+        <v>56</v>
+      </c>
+      <c r="H4" s="37">
+        <v>57</v>
+      </c>
+      <c r="I4" s="38">
+        <v>58</v>
+      </c>
+      <c r="J4" s="123">
+        <v>59</v>
+      </c>
+      <c r="L4" s="29">
+        <v>5</v>
+      </c>
+      <c r="M4" s="30">
+        <v>7</v>
+      </c>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+    </row>
+    <row r="5" spans="1:15" ht="30" customHeight="1">
+      <c r="A5" s="2"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="75"/>
+      <c r="L5" s="31">
+        <v>15</v>
+      </c>
+      <c r="M5" s="30">
+        <v>17</v>
+      </c>
+      <c r="N5" s="30"/>
+      <c r="O5" s="30"/>
+    </row>
+    <row r="6" spans="1:15" ht="30" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="120">
+        <v>47</v>
+      </c>
+      <c r="C6" s="10">
+        <v>48</v>
+      </c>
+      <c r="D6" s="126">
+        <v>49</v>
+      </c>
+      <c r="E6" s="121" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J6" s="74" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="32">
+        <v>9</v>
+      </c>
+      <c r="M6" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="N6" s="30"/>
+      <c r="O6" s="30"/>
+    </row>
+    <row r="7" spans="1:15" ht="30" customHeight="1" thickBot="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="125"/>
+      <c r="E7" s="128" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="122" t="s">
+        <v>75</v>
+      </c>
+      <c r="G7" s="129" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="122" t="s">
+        <v>77</v>
+      </c>
+      <c r="I7" s="130" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" s="75"/>
+      <c r="L7" s="33">
+        <v>22</v>
+      </c>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+    </row>
+    <row r="8" spans="1:15" ht="30" customHeight="1">
+      <c r="B8" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="16">
+        <v>40</v>
+      </c>
+      <c r="F8" s="25">
+        <v>41</v>
+      </c>
+      <c r="G8" s="36">
+        <v>42</v>
+      </c>
+      <c r="H8" s="16">
+        <v>43</v>
+      </c>
+      <c r="I8" s="43">
+        <v>44</v>
+      </c>
+      <c r="J8" s="76">
+        <v>45</v>
+      </c>
+      <c r="L8" s="30">
+        <v>3</v>
+      </c>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="30"/>
+    </row>
+    <row r="9" spans="1:15" ht="30" customHeight="1" thickBot="1">
+      <c r="A9" s="2"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="135" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="93" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
+      <c r="O9" s="30"/>
+    </row>
+    <row r="10" spans="1:15" ht="30" customHeight="1">
+      <c r="A10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="39">
+        <v>33</v>
+      </c>
+      <c r="C10" s="40">
+        <v>34</v>
+      </c>
+      <c r="D10" s="40">
+        <v>35</v>
+      </c>
+      <c r="E10" s="40">
+        <v>36</v>
+      </c>
+      <c r="F10" s="44">
+        <v>37</v>
+      </c>
+      <c r="G10" s="131">
+        <v>38</v>
+      </c>
+      <c r="H10" s="136">
+        <v>39</v>
+      </c>
+      <c r="I10" s="137" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="140" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
+      <c r="O10" s="30"/>
+    </row>
+    <row r="11" spans="1:15" ht="30" customHeight="1">
+      <c r="A11" s="2"/>
+      <c r="B11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="132"/>
+      <c r="H11" s="117" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="109" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="141" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="30"/>
+    </row>
+    <row r="12" spans="1:15" ht="30" customHeight="1">
+      <c r="A12" s="2"/>
+      <c r="B12" s="12">
+        <v>29</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="46" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="133" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="118" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="106">
+        <v>30</v>
+      </c>
+      <c r="J12" s="142">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="30" customHeight="1" thickBot="1">
+      <c r="A13" s="2"/>
+      <c r="B13" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="134"/>
+      <c r="H13" s="138" t="s">
+        <v>66</v>
+      </c>
+      <c r="I13" s="139" t="s">
+        <v>67</v>
+      </c>
+      <c r="J13" s="143" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="30" customHeight="1">
+      <c r="A14" s="2"/>
+      <c r="B14" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="16">
+        <v>20</v>
+      </c>
+      <c r="D14" s="25">
+        <v>21</v>
+      </c>
+      <c r="E14" s="34">
+        <v>22</v>
+      </c>
+      <c r="F14" s="16">
+        <v>23</v>
+      </c>
+      <c r="G14" s="36">
+        <v>24</v>
+      </c>
+      <c r="H14" s="16">
+        <v>25</v>
+      </c>
+      <c r="I14" s="43">
+        <v>26</v>
+      </c>
+      <c r="J14" s="51">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="30" customHeight="1" thickBot="1">
+      <c r="A15" s="2"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="51"/>
+    </row>
+    <row r="16" spans="1:15" ht="30" customHeight="1">
+      <c r="A16" s="2"/>
+      <c r="B16" s="89">
+        <v>15</v>
+      </c>
+      <c r="C16" s="53">
+        <v>16</v>
+      </c>
+      <c r="D16" s="54">
+        <v>17</v>
+      </c>
+      <c r="E16" s="81">
+        <v>18</v>
+      </c>
+      <c r="F16" s="52">
+        <v>19</v>
+      </c>
+      <c r="G16" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="88" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" customHeight="1">
+      <c r="A17" s="2"/>
+      <c r="B17" s="90" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="82"/>
+      <c r="F17" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="J17" s="78" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" customHeight="1">
+      <c r="A18" s="2"/>
+      <c r="B18" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" s="83" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="62">
+        <v>10</v>
+      </c>
+      <c r="H18" s="10">
+        <v>11</v>
+      </c>
+      <c r="I18" s="63">
+        <v>12</v>
+      </c>
+      <c r="J18" s="79">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" customHeight="1" thickBot="1">
+      <c r="A19" s="2"/>
+      <c r="B19" s="92" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="84"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="64" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="20"/>
+      <c r="I19" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="J19" s="80" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>